<commit_message>
Commit to move NB Reports fixes from branch 'corp_meetings' into master
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_USD_2.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_USD_2.xlsx
@@ -741,11 +741,11 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="8" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B9" sqref="B9"/>
       <selection pane="topRight" activeCell="B9" sqref="B9"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:F4"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>